<commit_message>
Import products by branch in all formats
</commit_message>
<xml_diff>
--- a/public/upload/catalog/upload-sample.xlsx
+++ b/public/upload/catalog/upload-sample.xlsx
@@ -27,9 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>name</t>
+    <t>branch_name</t>
+  </si>
+  <si>
+    <t>product_name</t>
   </si>
   <si>
     <t>quantity</t>
@@ -1025,19 +1028,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="10.1818181818182" customWidth="1"/>
-    <col min="4" max="4" width="11.8181818181818" customWidth="1"/>
+    <col min="1" max="1" width="13.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="14.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="11.8181818181818" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,6 +1057,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
orders flow updated,Payment Methods & Import fields added
</commit_message>
<xml_diff>
--- a/public/upload/catalog/upload-sample.xlsx
+++ b/public/upload/catalog/upload-sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19190" windowHeight="8730"/>
+    <workbookView windowWidth="16270" windowHeight="5450"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>branch_name</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>expire_date</t>
   </si>
   <si>
     <t>price</t>
@@ -1028,20 +1034,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="13.5454545454545" customWidth="1"/>
     <col min="2" max="2" width="14.4545454545455" customWidth="1"/>
     <col min="5" max="5" width="11.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="11.8181818181818" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,6 +1067,12 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed upload sample doc
</commit_message>
<xml_diff>
--- a/public/upload/catalog/upload-sample.xlsx
+++ b/public/upload/catalog/upload-sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="16270" windowHeight="5450"/>
+    <workbookView windowWidth="19190" windowHeight="7520"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>branch_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>product_name</t>
   </si>
@@ -1034,21 +1031,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.5454545454545" customWidth="1"/>
-    <col min="2" max="2" width="14.4545454545455" customWidth="1"/>
-    <col min="5" max="5" width="11.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="11.8181818181818" customWidth="1"/>
+    <col min="1" max="1" width="14.4545454545455" customWidth="1"/>
+    <col min="4" max="4" width="11.8181818181818" customWidth="1"/>
+    <col min="6" max="6" width="11.8181818181818" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1070,9 +1066,6 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>